<commit_message>
Updated Based on TGOLD's Suggestions
</commit_message>
<xml_diff>
--- a/Docs/TimeLine.xlsx
+++ b/Docs/TimeLine.xlsx
@@ -653,7 +653,7 @@
     <cellStyle name="Project Headers" xfId="4"/>
     <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="18">
     <dxf>
       <fill>
         <patternFill>
@@ -794,119 +794,6 @@
         </top>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1268,18 +1155,18 @@
   </sheetPr>
   <dimension ref="A1:CD23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="43" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <pane xSplit="5" topLeftCell="AG1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CD8" sqref="CD8"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="42" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <pane xSplit="5" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="72.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="33.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="24.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="35.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="33.88671875" style="1" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="35.109375" style="1" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="20.6640625" style="4" customWidth="1"/>
     <col min="7" max="26" width="5.77734375" style="1" customWidth="1"/>
     <col min="27" max="67" width="5.77734375" customWidth="1"/>
@@ -1287,7 +1174,7 @@
     <col min="70" max="82" width="5.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:82" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.05">
+    <row r="1" spans="1:82" ht="54.6" customHeight="1" x14ac:dyDescent="1">
       <c r="A1" s="10"/>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -1313,7 +1200,7 @@
       <c r="U1" s="21"/>
       <c r="V1" s="21"/>
     </row>
-    <row r="2" spans="1:82" ht="34.799999999999997" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:82" ht="51.6" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="28"/>
       <c r="B2" s="28"/>
       <c r="C2" s="28"/>
@@ -1369,7 +1256,7 @@
       <c r="AN2" s="27"/>
       <c r="AO2" s="27"/>
     </row>
-    <row r="3" spans="1:82" s="8" customFormat="1" ht="61.8" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:82" s="8" customFormat="1" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>0</v>
       </c>
@@ -1617,7 +1504,7 @@
         <v>43066</v>
       </c>
     </row>
-    <row r="4" spans="1:82" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:82" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30"/>
       <c r="B4" s="32"/>
       <c r="C4" s="32"/>
@@ -2194,13 +2081,13 @@
         <v>30</v>
       </c>
       <c r="B21" s="5">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C21" s="5">
         <v>1</v>
       </c>
       <c r="D21" s="5">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="E21" s="5">
         <v>1</v>

</xml_diff>